<commit_message>
Fixed all Auto Complete on Forms
Related Work Items: #46, #70, #81
</commit_message>
<xml_diff>
--- a/HCL_HRIS/Files/Excel_Templates/Audit_Template.xlsx
+++ b/HCL_HRIS/Files/Excel_Templates/Audit_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristianJohn.Banal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristianJohn.Banal\source\repos\HCL_HRIS\HCL_HRIS\Files\Excel_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Case ID</t>
   </si>
@@ -44,9 +44,6 @@
     <t>CC</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Fatal</t>
   </si>
   <si>
@@ -56,34 +53,16 @@
     <t>Date Of Transaction</t>
   </si>
   <si>
-    <t>Qulaity123456</t>
-  </si>
-  <si>
-    <t>Qulaity456789</t>
-  </si>
-  <si>
     <t>Audit Type</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>Non SLA</t>
   </si>
   <si>
     <t>Type of Monitoring</t>
   </si>
   <si>
-    <t>Recorded Monitoring</t>
+    <t>Note:</t>
   </si>
   <si>
-    <t>Side by Side Monitoring</t>
-  </si>
-  <si>
-    <t>MIP</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>For BC, EUC, CC or Fatal. Please use "Pass" or "Fail".</t>
   </si>
 </sst>
 </file>
@@ -237,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +256,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -578,19 +563,21 @@
     <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.7109375" style="1" customWidth="1"/>
     <col min="6" max="7" width="17.7109375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -599,10 +586,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -614,115 +601,55 @@
         <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4">
-        <v>51695613</v>
-      </c>
-      <c r="E2" s="4">
-        <v>51787452</v>
-      </c>
-      <c r="F2" s="5">
-        <v>43810</v>
-      </c>
-      <c r="G2" s="5">
-        <v>43809</v>
-      </c>
-      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
+      <c r="M1" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>51695613</v>
-      </c>
-      <c r="E3" s="7">
-        <v>51797122</v>
-      </c>
-      <c r="F3" s="8">
-        <v>43810</v>
-      </c>
-      <c r="G3" s="8">
-        <v>43809</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7">
-        <v>51695613</v>
-      </c>
-      <c r="E4" s="7">
-        <v>51797122</v>
-      </c>
-      <c r="F4" s="8">
-        <v>43810</v>
-      </c>
-      <c r="G4" s="8">
-        <v>43809</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -735,7 +662,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -748,7 +675,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -761,7 +688,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -774,7 +701,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -787,7 +714,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -800,7 +727,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -813,7 +740,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -826,7 +753,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -839,7 +766,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -852,7 +779,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -865,7 +792,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>

</xml_diff>